<commit_message>
Pin de colores en mapas
</commit_message>
<xml_diff>
--- a/Pantallas.xlsx
+++ b/Pantallas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\fleetdeliveryapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F00ADC-CC66-4EEB-A31B-8E35347E571B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBF5A29-0110-4860-90E9-2A7D0BA8B18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{019D86E0-0366-443C-B361-9E92F2872354}"/>
   </bookViews>
@@ -1858,8 +1858,8 @@
   <dimension ref="A1:T265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C119" sqref="C119:I119"/>
+      <pane ySplit="4" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K123" sqref="K123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Cambios 2 de mayo
</commit_message>
<xml_diff>
--- a/Pantallas.xlsx
+++ b/Pantallas.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\fleetdeliveryapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C176EC-EB13-4730-AE0C-27698C0FB806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B228729-2425-459E-AF94-D53F8C532E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{019D86E0-0366-443C-B361-9E92F2872354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{019D86E0-0366-443C-B361-9E92F2872354}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Pablo 22Abril" sheetId="3" r:id="rId3"/>
     <sheet name="Lo que pide Fleet" sheetId="4" r:id="rId4"/>
+    <sheet name="OPCIONES" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="275">
   <si>
     <t>Controles Remotos</t>
   </si>
@@ -636,12 +637,284 @@
   <si>
     <t xml:space="preserve">  Tuve que poner en la Tabla CodigosCierresAsignaciones la fila TLC Codigo 45</t>
   </si>
+  <si>
+    <t>Cant. Registros</t>
+  </si>
+  <si>
+    <t>Acción</t>
+  </si>
+  <si>
+    <t>SI (Recuperado/Entregado)</t>
+  </si>
+  <si>
+    <t>NO (No recuperado/No entregado)</t>
+  </si>
+  <si>
+    <t>Más de 1</t>
+  </si>
+  <si>
+    <t>Todos SI (Recuperados/Entregados)</t>
+  </si>
+  <si>
+    <t>Todos NO (No recuperados/No entregados)</t>
+  </si>
+  <si>
+    <t>Algunos SI y algunos NO</t>
+  </si>
+  <si>
+    <t>ESTADOGAOS</t>
+  </si>
+  <si>
+    <t>EJB</t>
+  </si>
+  <si>
+    <t>INC</t>
+  </si>
+  <si>
+    <t>Al menos 6 dígitos</t>
+  </si>
+  <si>
+    <t>TelefAlternativo4</t>
+  </si>
+  <si>
+    <t>TelefAlternativo3</t>
+  </si>
+  <si>
+    <t>TelefAlternativo2</t>
+  </si>
+  <si>
+    <t>TelefAlternativo1</t>
+  </si>
+  <si>
+    <t>MedioCit</t>
+  </si>
+  <si>
+    <t>FechaCit</t>
+  </si>
+  <si>
+    <t>FechaEvento1</t>
+  </si>
+  <si>
+    <t>Evento1</t>
+  </si>
+  <si>
+    <t>FechaEvento2</t>
+  </si>
+  <si>
+    <t>Evento2</t>
+  </si>
+  <si>
+    <t>FechaEvento3</t>
+  </si>
+  <si>
+    <t>Evento3</t>
+  </si>
+  <si>
+    <t>FechaEvento4</t>
+  </si>
+  <si>
+    <t>Evento4</t>
+  </si>
+  <si>
+    <t>Motivos</t>
+  </si>
+  <si>
+    <t>MODELO</t>
+  </si>
+  <si>
+    <t>ReclamoTecnicoID</t>
+  </si>
+  <si>
+    <t>ObservacionCaptura</t>
+  </si>
+  <si>
+    <t>HsCumplidaTime</t>
+  </si>
+  <si>
+    <t>CantRem</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>HsCumplida</t>
+  </si>
+  <si>
+    <t>PROYECTOMODULO</t>
+  </si>
+  <si>
+    <t>FechaAsignada</t>
+  </si>
+  <si>
+    <t>CAUSANTEC</t>
+  </si>
+  <si>
+    <t>SUBCON</t>
+  </si>
+  <si>
+    <t>FECHACUMPLIDA</t>
+  </si>
+  <si>
+    <t>ZONA</t>
+  </si>
+  <si>
+    <t>UrlFirma</t>
+  </si>
+  <si>
+    <t>UrlDni</t>
+  </si>
+  <si>
+    <t>ImageArrayFirma</t>
+  </si>
+  <si>
+    <t>ImageArrayDni</t>
+  </si>
+  <si>
+    <t>ESTADO2</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>GRYY</t>
+  </si>
+  <si>
+    <t>GRXX</t>
+  </si>
+  <si>
+    <t>TELEFONO</t>
+  </si>
+  <si>
+    <t>PROVINCIA</t>
+  </si>
+  <si>
+    <t>LOCALIDAD</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>ENTRECALLE2</t>
+  </si>
+  <si>
+    <t>ENTRECALLE1</t>
+  </si>
+  <si>
+    <t>DOMICILIO</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>RECUPIDJOBCARD</t>
+  </si>
+  <si>
+    <t>IDREGISTRO</t>
+  </si>
+  <si>
+    <t>DateTime.now()</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Foto DNI</t>
+  </si>
+  <si>
+    <t>Firma</t>
+  </si>
+  <si>
+    <t>Formato ENTERO</t>
+  </si>
+  <si>
+    <t>Ver con Pablo</t>
+  </si>
+  <si>
+    <t>El que corresponda según el ProyectoModulo</t>
+  </si>
+  <si>
+    <t>A elección en la APP</t>
+  </si>
+  <si>
+    <t>De acá a la derecha son campos que deben mantener el valor que tenìan</t>
+  </si>
+  <si>
+    <t>Descripción del Cód. de Cierre</t>
+  </si>
+  <si>
+    <t>lat min</t>
+  </si>
+  <si>
+    <t>lat max</t>
+  </si>
+  <si>
+    <t>longin</t>
+  </si>
+  <si>
+    <t>longmax</t>
+  </si>
+  <si>
+    <t>latpro</t>
+  </si>
+  <si>
+    <t>longprom</t>
+  </si>
+  <si>
+    <t>AL tocar el mapa sin elegir asignaciones da error</t>
+  </si>
+  <si>
+    <r>
+      <t>Agregar Antigüedad (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>días</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y sacarle el decimal</t>
+    </r>
+  </si>
+  <si>
+    <t>Leer en Tabla FuncionesApps si es obligatorio</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>HGU 004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queda lo que había salvo que elija de la lista desplegable. </t>
+  </si>
+  <si>
+    <t>que guardaría DECO1 de lo que se eligió en la lista desplegable</t>
+  </si>
+  <si>
+    <t>La Obs de la APP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -698,8 +971,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,6 +1047,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -794,7 +1093,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -823,11 +1122,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1845,6 +2162,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1051560</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>109166</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{735E9C4E-80B3-F068-2614-25D099C204FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="403860" y="3314700"/>
+          <a:ext cx="1424940" cy="1869386"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -2145,8 +2528,8 @@
   <dimension ref="A1:T269"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H130" sqref="H130"/>
+      <pane ySplit="4" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C123" sqref="C123:K123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2254,76 +2637,76 @@
       <c r="A92" s="8"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A93" s="22" t="s">
+      <c r="A93" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B93" s="22"/>
-      <c r="C93" s="22"/>
-      <c r="D93" s="22" t="s">
+      <c r="B93" s="32"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="E93" s="22"/>
-      <c r="F93" s="22"/>
-      <c r="G93" s="22" t="s">
+      <c r="E93" s="32"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="H93" s="22"/>
-      <c r="I93" s="22"/>
-      <c r="J93" s="22" t="s">
+      <c r="H93" s="32"/>
+      <c r="I93" s="32"/>
+      <c r="J93" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K93" s="22"/>
-      <c r="L93" s="22"/>
-      <c r="M93" s="22" t="s">
+      <c r="K93" s="32"/>
+      <c r="L93" s="32"/>
+      <c r="M93" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="N93" s="22"/>
-      <c r="O93" s="22"/>
-      <c r="P93" s="22" t="s">
+      <c r="N93" s="32"/>
+      <c r="O93" s="32"/>
+      <c r="P93" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="Q93" s="22"/>
-      <c r="R93" s="22"/>
+      <c r="Q93" s="32"/>
+      <c r="R93" s="32"/>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A94" s="22"/>
-      <c r="B94" s="22"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="22"/>
-      <c r="I94" s="22"/>
-      <c r="J94" s="22"/>
-      <c r="K94" s="22"/>
-      <c r="L94" s="22"/>
-      <c r="M94" s="22"/>
-      <c r="N94" s="22"/>
-      <c r="O94" s="22"/>
-      <c r="P94" s="22"/>
-      <c r="Q94" s="22"/>
-      <c r="R94" s="22"/>
+      <c r="A94" s="32"/>
+      <c r="B94" s="32"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="32"/>
+      <c r="E94" s="32"/>
+      <c r="F94" s="32"/>
+      <c r="G94" s="32"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="32"/>
+      <c r="J94" s="32"/>
+      <c r="K94" s="32"/>
+      <c r="L94" s="32"/>
+      <c r="M94" s="32"/>
+      <c r="N94" s="32"/>
+      <c r="O94" s="32"/>
+      <c r="P94" s="32"/>
+      <c r="Q94" s="32"/>
+      <c r="R94" s="32"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A95" s="22"/>
-      <c r="B95" s="22"/>
-      <c r="C95" s="22"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="22"/>
-      <c r="F95" s="22"/>
-      <c r="G95" s="22"/>
-      <c r="H95" s="22"/>
-      <c r="I95" s="22"/>
-      <c r="J95" s="22"/>
-      <c r="K95" s="22"/>
-      <c r="L95" s="22"/>
-      <c r="M95" s="22"/>
-      <c r="N95" s="22"/>
-      <c r="O95" s="22"/>
-      <c r="P95" s="22"/>
-      <c r="Q95" s="22"/>
-      <c r="R95" s="22"/>
+      <c r="A95" s="32"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="32"/>
+      <c r="G95" s="32"/>
+      <c r="H95" s="32"/>
+      <c r="I95" s="32"/>
+      <c r="J95" s="32"/>
+      <c r="K95" s="32"/>
+      <c r="L95" s="32"/>
+      <c r="M95" s="32"/>
+      <c r="N95" s="32"/>
+      <c r="O95" s="32"/>
+      <c r="P95" s="32"/>
+      <c r="Q95" s="32"/>
+      <c r="R95" s="32"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G96" s="9"/>
@@ -4313,15 +4696,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D88255-D2CC-4409-89E6-047B710929E7}">
-  <dimension ref="F2:N25"/>
+  <dimension ref="F1:P42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:M5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
         <v>149</v>
       </c>
@@ -4331,8 +4722,14 @@
       <c r="H2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="3" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="O2">
+        <v>213123123</v>
+      </c>
+      <c r="P2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F3" t="s">
         <v>97</v>
       </c>
@@ -4349,7 +4746,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="6:16" x14ac:dyDescent="0.3">
       <c r="H5" s="20" t="s">
         <v>154</v>
       </c>
@@ -4359,7 +4756,7 @@
       <c r="L5" s="20"/>
       <c r="M5" s="20"/>
     </row>
-    <row r="9" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="6:16" x14ac:dyDescent="0.3">
       <c r="H9" s="20" t="s">
         <v>155</v>
       </c>
@@ -4372,7 +4769,7 @@
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
     </row>
-    <row r="10" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:16" x14ac:dyDescent="0.3">
       <c r="H10" s="20"/>
       <c r="I10" s="20" t="s">
         <v>156</v>
@@ -4385,7 +4782,7 @@
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
     </row>
-    <row r="11" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="6:16" x14ac:dyDescent="0.3">
       <c r="H11" s="20"/>
       <c r="I11" s="20" t="s">
         <v>157</v>
@@ -4398,7 +4795,7 @@
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
     </row>
-    <row r="12" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="6:16" x14ac:dyDescent="0.3">
       <c r="H12" s="20"/>
       <c r="I12" s="20" t="s">
         <v>158</v>
@@ -4413,7 +4810,7 @@
       </c>
       <c r="N12" s="20"/>
     </row>
-    <row r="13" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="6:16" x14ac:dyDescent="0.3">
       <c r="H13" s="20"/>
       <c r="I13" s="20" t="s">
         <v>159</v>
@@ -4426,7 +4823,7 @@
       <c r="M13" s="20"/>
       <c r="N13" s="20"/>
     </row>
-    <row r="16" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="6:16" x14ac:dyDescent="0.3">
       <c r="H16" s="20" t="s">
         <v>189</v>
       </c>
@@ -4440,7 +4837,7 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="22" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4460,8 +4857,53 @@
       </c>
     </row>
     <row r="25" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H25" t="s">
+      <c r="H25" s="31" t="s">
         <v>190</v>
+      </c>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="27" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H27" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+    </row>
+    <row r="29" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H29" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>262</v>
+      </c>
+      <c r="I39" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>264</v>
+      </c>
+      <c r="I42" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -4475,8 +4917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6A065A-E9FC-4057-A0DA-97BEAEB3828B}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4514,7 +4956,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>182</v>
       </c>
       <c r="B5" t="s">
@@ -4522,7 +4964,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>182</v>
       </c>
       <c r="B6" t="s">
@@ -4609,4 +5051,1770 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD34139A-7E06-4758-A327-67E7555E57FF}">
+  <dimension ref="A1:BH31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.21875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="48.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.88671875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="58" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="16384" width="11.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="P5" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="S5" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="T5" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="U5" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="V5" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="W5" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y5" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z5" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA5" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB5" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC5" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD5" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="AE5" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF5" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AG5" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH5" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI5" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="AJ5" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="AK5" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL5" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="AM5" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN5" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="AO5" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="AP5" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="AQ5" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="AR5" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="AS5" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="AT5" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU5" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="AV5" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="AW5" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="AX5" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="AY5" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="AZ5" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="BA5" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="BB5" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="BC5" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="BD5" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="BE5" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="BF5" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="BG5" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="BH5" s="27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>1</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="11"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="11"/>
+      <c r="AR6" s="11"/>
+      <c r="AS6" s="11"/>
+      <c r="AT6" s="11"/>
+      <c r="AU6" s="11"/>
+      <c r="AV6" s="11"/>
+      <c r="AW6" s="11"/>
+      <c r="AX6" s="11"/>
+      <c r="AY6" s="11"/>
+      <c r="AZ6" s="11"/>
+      <c r="BA6" s="11"/>
+      <c r="BB6" s="11"/>
+      <c r="BC6" s="11"/>
+      <c r="BD6" s="11"/>
+      <c r="BE6" s="11"/>
+      <c r="BF6" s="11"/>
+      <c r="BG6" s="11"/>
+      <c r="BH6" s="11"/>
+    </row>
+    <row r="8" spans="1:60" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="28"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="28"/>
+      <c r="AF8" s="28"/>
+      <c r="AG8" s="28"/>
+      <c r="AH8" s="28"/>
+      <c r="AI8" s="28"/>
+      <c r="AJ8" s="28"/>
+      <c r="AK8" s="28"/>
+      <c r="AL8" s="28"/>
+      <c r="AM8" s="28"/>
+      <c r="AN8" s="28"/>
+      <c r="AO8" s="28"/>
+      <c r="AP8" s="28"/>
+      <c r="AQ8" s="28"/>
+      <c r="AR8" s="28"/>
+      <c r="AS8" s="28"/>
+      <c r="AT8" s="28"/>
+      <c r="AU8" s="28"/>
+      <c r="AV8" s="28"/>
+      <c r="AW8" s="28"/>
+      <c r="AX8" s="28"/>
+      <c r="AY8" s="28"/>
+      <c r="AZ8" s="28"/>
+      <c r="BA8" s="28"/>
+      <c r="BB8" s="28"/>
+      <c r="BC8" s="28"/>
+      <c r="BD8" s="28"/>
+      <c r="BE8" s="28"/>
+      <c r="BF8" s="28"/>
+      <c r="BG8" s="28"/>
+      <c r="BH8" s="28"/>
+    </row>
+    <row r="10" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A10" s="25">
+        <v>1</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="11"/>
+      <c r="AM10" s="11"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="11"/>
+      <c r="AP10" s="11"/>
+      <c r="AQ10" s="11"/>
+      <c r="AR10" s="11"/>
+      <c r="AS10" s="11"/>
+      <c r="AT10" s="11"/>
+      <c r="AU10" s="11"/>
+      <c r="AV10" s="11"/>
+      <c r="AW10" s="11"/>
+      <c r="AX10" s="11"/>
+      <c r="AY10" s="11"/>
+      <c r="AZ10" s="11"/>
+      <c r="BA10" s="11"/>
+      <c r="BB10" s="11"/>
+      <c r="BC10" s="11"/>
+      <c r="BD10" s="11"/>
+      <c r="BE10" s="11"/>
+      <c r="BF10" s="11"/>
+      <c r="BG10" s="11"/>
+      <c r="BH10" s="11"/>
+    </row>
+    <row r="12" spans="1:60" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="28"/>
+      <c r="AC12" s="28"/>
+      <c r="AD12" s="28"/>
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="28"/>
+      <c r="AG12" s="28"/>
+      <c r="AH12" s="28"/>
+      <c r="AI12" s="28"/>
+      <c r="AJ12" s="28"/>
+      <c r="AK12" s="28"/>
+      <c r="AL12" s="28"/>
+      <c r="AM12" s="28"/>
+      <c r="AN12" s="28"/>
+      <c r="AO12" s="28"/>
+      <c r="AP12" s="28"/>
+      <c r="AQ12" s="28"/>
+      <c r="AR12" s="28"/>
+      <c r="AS12" s="28"/>
+      <c r="AT12" s="28"/>
+      <c r="AU12" s="28"/>
+      <c r="AV12" s="28"/>
+      <c r="AW12" s="28"/>
+      <c r="AX12" s="28"/>
+      <c r="AY12" s="28"/>
+      <c r="AZ12" s="28"/>
+      <c r="BA12" s="28"/>
+      <c r="BB12" s="28"/>
+      <c r="BC12" s="28"/>
+      <c r="BD12" s="28"/>
+      <c r="BE12" s="28"/>
+      <c r="BF12" s="28"/>
+      <c r="BG12" s="28"/>
+      <c r="BH12" s="28"/>
+    </row>
+    <row r="14" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="11"/>
+      <c r="AM14" s="11"/>
+      <c r="AN14" s="11"/>
+      <c r="AO14" s="11"/>
+      <c r="AP14" s="11"/>
+      <c r="AQ14" s="11"/>
+      <c r="AR14" s="11"/>
+      <c r="AS14" s="11"/>
+      <c r="AT14" s="11"/>
+      <c r="AU14" s="11"/>
+      <c r="AV14" s="11"/>
+      <c r="AW14" s="11"/>
+      <c r="AX14" s="11"/>
+      <c r="AY14" s="11"/>
+      <c r="AZ14" s="11"/>
+      <c r="BA14" s="11"/>
+      <c r="BB14" s="11"/>
+      <c r="BC14" s="11"/>
+      <c r="BD14" s="11"/>
+      <c r="BE14" s="11"/>
+      <c r="BF14" s="11"/>
+      <c r="BG14" s="11"/>
+      <c r="BH14" s="11"/>
+    </row>
+    <row r="15" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C15" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="11"/>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="11"/>
+      <c r="AM15" s="11"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
+      <c r="AQ15" s="11"/>
+      <c r="AR15" s="11"/>
+      <c r="AS15" s="11"/>
+      <c r="AT15" s="11"/>
+      <c r="AU15" s="11"/>
+      <c r="AV15" s="11"/>
+      <c r="AW15" s="11"/>
+      <c r="AX15" s="11"/>
+      <c r="AY15" s="11"/>
+      <c r="AZ15" s="11"/>
+      <c r="BA15" s="11"/>
+      <c r="BB15" s="11"/>
+      <c r="BC15" s="11"/>
+      <c r="BD15" s="11"/>
+      <c r="BE15" s="11"/>
+      <c r="BF15" s="11"/>
+      <c r="BG15" s="11"/>
+      <c r="BH15" s="11"/>
+    </row>
+    <row r="16" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C16" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="11"/>
+      <c r="AM16" s="11"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="11"/>
+      <c r="AP16" s="11"/>
+      <c r="AQ16" s="11"/>
+      <c r="AR16" s="11"/>
+      <c r="AS16" s="11"/>
+      <c r="AT16" s="11"/>
+      <c r="AU16" s="11"/>
+      <c r="AV16" s="11"/>
+      <c r="AW16" s="11"/>
+      <c r="AX16" s="11"/>
+      <c r="AY16" s="11"/>
+      <c r="AZ16" s="11"/>
+      <c r="BA16" s="11"/>
+      <c r="BB16" s="11"/>
+      <c r="BC16" s="11"/>
+      <c r="BD16" s="11"/>
+      <c r="BE16" s="11"/>
+      <c r="BF16" s="11"/>
+      <c r="BG16" s="11"/>
+      <c r="BH16" s="11"/>
+    </row>
+    <row r="17" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C17" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11"/>
+      <c r="AF17" s="11"/>
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="11"/>
+      <c r="AI17" s="11"/>
+      <c r="AJ17" s="11"/>
+      <c r="AK17" s="11"/>
+      <c r="AL17" s="11"/>
+      <c r="AM17" s="11"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="11"/>
+      <c r="AP17" s="11"/>
+      <c r="AQ17" s="11"/>
+      <c r="AR17" s="11"/>
+      <c r="AS17" s="11"/>
+      <c r="AT17" s="11"/>
+      <c r="AU17" s="11"/>
+      <c r="AV17" s="11"/>
+      <c r="AW17" s="11"/>
+      <c r="AX17" s="11"/>
+      <c r="AY17" s="11"/>
+      <c r="AZ17" s="11"/>
+      <c r="BA17" s="11"/>
+      <c r="BB17" s="11"/>
+      <c r="BC17" s="11"/>
+      <c r="BD17" s="11"/>
+      <c r="BE17" s="11"/>
+      <c r="BF17" s="11"/>
+      <c r="BG17" s="11"/>
+      <c r="BH17" s="11"/>
+    </row>
+    <row r="19" spans="1:60" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="28"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="28"/>
+      <c r="AH19" s="28"/>
+      <c r="AI19" s="28"/>
+      <c r="AJ19" s="28"/>
+      <c r="AK19" s="28"/>
+      <c r="AL19" s="28"/>
+      <c r="AM19" s="28"/>
+      <c r="AN19" s="28"/>
+      <c r="AO19" s="28"/>
+      <c r="AP19" s="28"/>
+      <c r="AQ19" s="28"/>
+      <c r="AR19" s="28"/>
+      <c r="AS19" s="28"/>
+      <c r="AT19" s="28"/>
+      <c r="AU19" s="28"/>
+      <c r="AV19" s="28"/>
+      <c r="AW19" s="28"/>
+      <c r="AX19" s="28"/>
+      <c r="AY19" s="28"/>
+      <c r="AZ19" s="28"/>
+      <c r="BA19" s="28"/>
+      <c r="BB19" s="28"/>
+      <c r="BC19" s="28"/>
+      <c r="BD19" s="28"/>
+      <c r="BE19" s="28"/>
+      <c r="BF19" s="28"/>
+      <c r="BG19" s="28"/>
+      <c r="BH19" s="28"/>
+    </row>
+    <row r="21" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O21" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="11"/>
+      <c r="AK21" s="11"/>
+      <c r="AL21" s="11"/>
+      <c r="AM21" s="11"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="11"/>
+      <c r="AQ21" s="11"/>
+      <c r="AR21" s="11"/>
+      <c r="AS21" s="11"/>
+      <c r="AT21" s="11"/>
+      <c r="AU21" s="11"/>
+      <c r="AV21" s="11"/>
+      <c r="AW21" s="11"/>
+      <c r="AX21" s="11"/>
+      <c r="AY21" s="11"/>
+      <c r="AZ21" s="11"/>
+      <c r="BA21" s="11"/>
+      <c r="BB21" s="11"/>
+      <c r="BC21" s="11"/>
+      <c r="BD21" s="11"/>
+      <c r="BE21" s="11"/>
+      <c r="BF21" s="11"/>
+      <c r="BG21" s="11"/>
+      <c r="BH21" s="11"/>
+    </row>
+    <row r="22" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C22" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="11"/>
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="11"/>
+      <c r="AJ22" s="11"/>
+      <c r="AK22" s="11"/>
+      <c r="AL22" s="11"/>
+      <c r="AM22" s="11"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="11"/>
+      <c r="AQ22" s="11"/>
+      <c r="AR22" s="11"/>
+      <c r="AS22" s="11"/>
+      <c r="AT22" s="11"/>
+      <c r="AU22" s="11"/>
+      <c r="AV22" s="11"/>
+      <c r="AW22" s="11"/>
+      <c r="AX22" s="11"/>
+      <c r="AY22" s="11"/>
+      <c r="AZ22" s="11"/>
+      <c r="BA22" s="11"/>
+      <c r="BB22" s="11"/>
+      <c r="BC22" s="11"/>
+      <c r="BD22" s="11"/>
+      <c r="BE22" s="11"/>
+      <c r="BF22" s="11"/>
+      <c r="BG22" s="11"/>
+      <c r="BH22" s="11"/>
+    </row>
+    <row r="23" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C23" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="11"/>
+      <c r="AF23" s="11"/>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="11"/>
+      <c r="AI23" s="11"/>
+      <c r="AJ23" s="11"/>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="11"/>
+      <c r="AM23" s="11"/>
+      <c r="AN23" s="11"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="11"/>
+      <c r="AQ23" s="11"/>
+      <c r="AR23" s="11"/>
+      <c r="AS23" s="11"/>
+      <c r="AT23" s="11"/>
+      <c r="AU23" s="11"/>
+      <c r="AV23" s="11"/>
+      <c r="AW23" s="11"/>
+      <c r="AX23" s="11"/>
+      <c r="AY23" s="11"/>
+      <c r="AZ23" s="11"/>
+      <c r="BA23" s="11"/>
+      <c r="BB23" s="11"/>
+      <c r="BC23" s="11"/>
+      <c r="BD23" s="11"/>
+      <c r="BE23" s="11"/>
+      <c r="BF23" s="11"/>
+      <c r="BG23" s="11"/>
+      <c r="BH23" s="11"/>
+    </row>
+    <row r="24" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C24" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O24" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="11"/>
+      <c r="AF24" s="11"/>
+      <c r="AG24" s="11"/>
+      <c r="AH24" s="11"/>
+      <c r="AI24" s="11"/>
+      <c r="AJ24" s="11"/>
+      <c r="AK24" s="11"/>
+      <c r="AL24" s="11"/>
+      <c r="AM24" s="11"/>
+      <c r="AN24" s="11"/>
+      <c r="AO24" s="11"/>
+      <c r="AP24" s="11"/>
+      <c r="AQ24" s="11"/>
+      <c r="AR24" s="11"/>
+      <c r="AS24" s="11"/>
+      <c r="AT24" s="11"/>
+      <c r="AU24" s="11"/>
+      <c r="AV24" s="11"/>
+      <c r="AW24" s="11"/>
+      <c r="AX24" s="11"/>
+      <c r="AY24" s="11"/>
+      <c r="AZ24" s="11"/>
+      <c r="BA24" s="11"/>
+      <c r="BB24" s="11"/>
+      <c r="BC24" s="11"/>
+      <c r="BD24" s="11"/>
+      <c r="BE24" s="11"/>
+      <c r="BF24" s="11"/>
+      <c r="BG24" s="11"/>
+      <c r="BH24" s="11"/>
+    </row>
+    <row r="26" spans="1:60" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
+      <c r="S26" s="28"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="28"/>
+      <c r="X26" s="28"/>
+      <c r="Y26" s="28"/>
+      <c r="Z26" s="28"/>
+      <c r="AA26" s="28"/>
+      <c r="AB26" s="28"/>
+      <c r="AC26" s="28"/>
+      <c r="AD26" s="28"/>
+      <c r="AE26" s="28"/>
+      <c r="AF26" s="28"/>
+      <c r="AG26" s="28"/>
+      <c r="AH26" s="28"/>
+      <c r="AI26" s="28"/>
+      <c r="AJ26" s="28"/>
+      <c r="AK26" s="28"/>
+      <c r="AL26" s="28"/>
+      <c r="AM26" s="28"/>
+      <c r="AN26" s="28"/>
+      <c r="AO26" s="28"/>
+      <c r="AP26" s="28"/>
+      <c r="AQ26" s="28"/>
+      <c r="AR26" s="28"/>
+      <c r="AS26" s="28"/>
+      <c r="AT26" s="28"/>
+      <c r="AU26" s="28"/>
+      <c r="AV26" s="28"/>
+      <c r="AW26" s="28"/>
+      <c r="AX26" s="28"/>
+      <c r="AY26" s="28"/>
+      <c r="AZ26" s="28"/>
+      <c r="BA26" s="28"/>
+      <c r="BB26" s="28"/>
+      <c r="BC26" s="28"/>
+      <c r="BD26" s="28"/>
+      <c r="BE26" s="28"/>
+      <c r="BF26" s="28"/>
+      <c r="BG26" s="28"/>
+      <c r="BH26" s="28"/>
+    </row>
+    <row r="28" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A28" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O28" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+      <c r="AE28" s="11"/>
+      <c r="AF28" s="11"/>
+      <c r="AG28" s="11"/>
+      <c r="AH28" s="11"/>
+      <c r="AI28" s="11"/>
+      <c r="AJ28" s="11"/>
+      <c r="AK28" s="11"/>
+      <c r="AL28" s="11"/>
+      <c r="AM28" s="11"/>
+      <c r="AN28" s="11"/>
+      <c r="AO28" s="11"/>
+      <c r="AP28" s="11"/>
+      <c r="AQ28" s="11"/>
+      <c r="AR28" s="11"/>
+      <c r="AS28" s="11"/>
+      <c r="AT28" s="11"/>
+      <c r="AU28" s="11"/>
+      <c r="AV28" s="11"/>
+      <c r="AW28" s="11"/>
+      <c r="AX28" s="11"/>
+      <c r="AY28" s="11"/>
+      <c r="AZ28" s="11"/>
+      <c r="BA28" s="11"/>
+      <c r="BB28" s="11"/>
+      <c r="BC28" s="11"/>
+      <c r="BD28" s="11"/>
+      <c r="BE28" s="11"/>
+      <c r="BF28" s="11"/>
+      <c r="BG28" s="11"/>
+      <c r="BH28" s="11"/>
+    </row>
+    <row r="29" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C29" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N29" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O29" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="P29" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="11"/>
+      <c r="AE29" s="11"/>
+      <c r="AF29" s="11"/>
+      <c r="AG29" s="11"/>
+      <c r="AH29" s="11"/>
+      <c r="AI29" s="11"/>
+      <c r="AJ29" s="11"/>
+      <c r="AK29" s="11"/>
+      <c r="AL29" s="11"/>
+      <c r="AM29" s="11"/>
+      <c r="AN29" s="11"/>
+      <c r="AO29" s="11"/>
+      <c r="AP29" s="11"/>
+      <c r="AQ29" s="11"/>
+      <c r="AR29" s="11"/>
+      <c r="AS29" s="11"/>
+      <c r="AT29" s="11"/>
+      <c r="AU29" s="11"/>
+      <c r="AV29" s="11"/>
+      <c r="AW29" s="11"/>
+      <c r="AX29" s="11"/>
+      <c r="AY29" s="11"/>
+      <c r="AZ29" s="11"/>
+      <c r="BA29" s="11"/>
+      <c r="BB29" s="11"/>
+      <c r="BC29" s="11"/>
+      <c r="BD29" s="11"/>
+      <c r="BE29" s="11"/>
+      <c r="BF29" s="11"/>
+      <c r="BG29" s="11"/>
+      <c r="BH29" s="11"/>
+    </row>
+    <row r="30" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C30" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="11"/>
+      <c r="AD30" s="11"/>
+      <c r="AE30" s="11"/>
+      <c r="AF30" s="11"/>
+      <c r="AG30" s="11"/>
+      <c r="AH30" s="11"/>
+      <c r="AI30" s="11"/>
+      <c r="AJ30" s="11"/>
+      <c r="AK30" s="11"/>
+      <c r="AL30" s="11"/>
+      <c r="AM30" s="11"/>
+      <c r="AN30" s="11"/>
+      <c r="AO30" s="11"/>
+      <c r="AP30" s="11"/>
+      <c r="AQ30" s="11"/>
+      <c r="AR30" s="11"/>
+      <c r="AS30" s="11"/>
+      <c r="AT30" s="11"/>
+      <c r="AU30" s="11"/>
+      <c r="AV30" s="11"/>
+      <c r="AW30" s="11"/>
+      <c r="AX30" s="11"/>
+      <c r="AY30" s="11"/>
+      <c r="AZ30" s="11"/>
+      <c r="BA30" s="11"/>
+      <c r="BB30" s="11"/>
+      <c r="BC30" s="11"/>
+      <c r="BD30" s="11"/>
+      <c r="BE30" s="11"/>
+      <c r="BF30" s="11"/>
+      <c r="BG30" s="11"/>
+      <c r="BH30" s="11"/>
+    </row>
+    <row r="31" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="C31" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O31" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P31" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="11"/>
+      <c r="AF31" s="11"/>
+      <c r="AG31" s="11"/>
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="11"/>
+      <c r="AJ31" s="11"/>
+      <c r="AK31" s="11"/>
+      <c r="AL31" s="11"/>
+      <c r="AM31" s="11"/>
+      <c r="AN31" s="11"/>
+      <c r="AO31" s="11"/>
+      <c r="AP31" s="11"/>
+      <c r="AQ31" s="11"/>
+      <c r="AR31" s="11"/>
+      <c r="AS31" s="11"/>
+      <c r="AT31" s="11"/>
+      <c r="AU31" s="11"/>
+      <c r="AV31" s="11"/>
+      <c r="AW31" s="11"/>
+      <c r="AX31" s="11"/>
+      <c r="AY31" s="11"/>
+      <c r="AZ31" s="11"/>
+      <c r="BA31" s="11"/>
+      <c r="BB31" s="11"/>
+      <c r="BC31" s="11"/>
+      <c r="BD31" s="11"/>
+      <c r="BE31" s="11"/>
+      <c r="BF31" s="11"/>
+      <c r="BG31" s="11"/>
+      <c r="BH31" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>